<commit_message>
플레이어 사격 동기화 완료 / Zombie_Manager, ZombieSpawnPoint 추가 / Zombie 생성 작업중
</commit_message>
<xml_diff>
--- a/졸작 진행 계획 시간표.xlsx
+++ b/졸작 진행 계획 시간표.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2020 졸작 깃\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA1F687-06AB-44ED-A916-385B553E145F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5B10E5-46A1-4C91-AB3F-9CD2FC711FCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E0805F39-A49F-47F5-8E79-FFCEB62D9AEC}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="108">
   <si>
     <t>월</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -472,10 +472,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>게임 내 시간 동기화 실제 적용 및 조정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2020. 06. 02. 화</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -484,11 +480,32 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>몬스터 객체 관리 송수신 패킷 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>몬스터 객체 정보 송수신 동기화</t>
+    <t>몬스터 관리 함수 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지정한 위치에 몬스터 생성하는 함수 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020. 06. 03. 수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>생성된 몬스터에 컨트롤러 빙의를 통한 비헤비어트리 적용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몬스터 관리를 위한 패킷정보 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몬스터 정보 패킷 송수신 함수 및 정보 갱신 함수 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몬스터 정보 패킷 송수신, 정보 갱신 함수 실제 적용 및 
+조정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1279,7 +1296,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="196">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1385,17 +1402,227 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1406,119 +1633,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1544,206 +1717,53 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1752,22 +1772,118 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2144,10 +2260,10 @@
       <c r="G5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="121" t="s">
+      <c r="H5" s="101" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="122"/>
+      <c r="I5" s="102"/>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.4">
@@ -2169,23 +2285,23 @@
       <c r="G6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="123"/>
-      <c r="I6" s="124"/>
+      <c r="H6" s="103"/>
+      <c r="I6" s="104"/>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="127" t="s">
+      <c r="C7" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="128"/>
-      <c r="E7" s="128"/>
-      <c r="F7" s="128"/>
-      <c r="G7" s="128"/>
-      <c r="H7" s="123"/>
-      <c r="I7" s="124"/>
+      <c r="D7" s="108"/>
+      <c r="E7" s="108"/>
+      <c r="F7" s="108"/>
+      <c r="G7" s="108"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="104"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -2207,8 +2323,8 @@
       <c r="G8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="123"/>
-      <c r="I8" s="124"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="104"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.4">
@@ -2230,8 +2346,8 @@
       <c r="G9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="123"/>
-      <c r="I9" s="124"/>
+      <c r="H9" s="103"/>
+      <c r="I9" s="104"/>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.4">
@@ -2253,8 +2369,8 @@
       <c r="G10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="123"/>
-      <c r="I10" s="124"/>
+      <c r="H10" s="103"/>
+      <c r="I10" s="104"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.4">
@@ -2276,8 +2392,8 @@
       <c r="G11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="123"/>
-      <c r="I11" s="124"/>
+      <c r="H11" s="103"/>
+      <c r="I11" s="104"/>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.4">
@@ -2299,8 +2415,8 @@
       <c r="G12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="123"/>
-      <c r="I12" s="124"/>
+      <c r="H12" s="103"/>
+      <c r="I12" s="104"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.45">
@@ -2322,8 +2438,8 @@
       <c r="G13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="125"/>
-      <c r="I13" s="126"/>
+      <c r="H13" s="105"/>
+      <c r="I13" s="106"/>
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.4">
@@ -2365,36 +2481,36 @@
       <c r="B17" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="93" t="s">
+      <c r="C17" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="94"/>
-      <c r="E17" s="94"/>
-      <c r="F17" s="94"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
       <c r="G17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="94" t="s">
+      <c r="H17" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="95"/>
+      <c r="I17" s="50"/>
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B18" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="96" t="s">
+      <c r="C18" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="97"/>
-      <c r="E18" s="97"/>
-      <c r="F18" s="98"/>
+      <c r="D18" s="85"/>
+      <c r="E18" s="85"/>
+      <c r="F18" s="86"/>
       <c r="G18" s="16">
         <v>1</v>
       </c>
-      <c r="H18" s="129"/>
-      <c r="I18" s="130"/>
+      <c r="H18" s="89"/>
+      <c r="I18" s="90"/>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.4">
@@ -2410,8 +2526,8 @@
       <c r="G19" s="16">
         <v>1</v>
       </c>
-      <c r="H19" s="72"/>
-      <c r="I19" s="73"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="42"/>
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.4">
@@ -2425,15 +2541,15 @@
       <c r="E20" s="37"/>
       <c r="F20" s="38"/>
       <c r="G20" s="16"/>
-      <c r="H20" s="72"/>
-      <c r="I20" s="73"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="42"/>
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B21" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="71" t="s">
+      <c r="C21" s="63" t="s">
         <v>31</v>
       </c>
       <c r="D21" s="37"/>
@@ -2442,8 +2558,8 @@
       <c r="G21" s="16">
         <v>1</v>
       </c>
-      <c r="H21" s="72"/>
-      <c r="I21" s="73"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="42"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B22" s="11" t="s">
@@ -2456,8 +2572,8 @@
       <c r="E22" s="37"/>
       <c r="F22" s="38"/>
       <c r="G22" s="16"/>
-      <c r="H22" s="72"/>
-      <c r="I22" s="73"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="42"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B23" s="11" t="s">
@@ -2470,8 +2586,8 @@
       <c r="E23" s="37"/>
       <c r="F23" s="38"/>
       <c r="G23" s="16"/>
-      <c r="H23" s="72"/>
-      <c r="I23" s="73"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="42"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B24" s="11" t="s">
@@ -2486,8 +2602,8 @@
       <c r="G24" s="16">
         <v>1</v>
       </c>
-      <c r="H24" s="72"/>
-      <c r="I24" s="73"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="42"/>
     </row>
     <row r="25" spans="2:10" ht="51" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B25" s="11" t="s">
@@ -2502,59 +2618,59 @@
       <c r="G25" s="16">
         <v>0.8</v>
       </c>
-      <c r="H25" s="119" t="s">
+      <c r="H25" s="114" t="s">
         <v>38</v>
       </c>
-      <c r="I25" s="120"/>
+      <c r="I25" s="115"/>
     </row>
     <row r="26" spans="2:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B26" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="39" t="s">
+      <c r="C26" s="109" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="41"/>
+      <c r="D26" s="110"/>
+      <c r="E26" s="110"/>
+      <c r="F26" s="111"/>
       <c r="G26" s="17">
         <v>1</v>
       </c>
-      <c r="H26" s="117"/>
-      <c r="I26" s="118"/>
+      <c r="H26" s="112"/>
+      <c r="I26" s="113"/>
     </row>
     <row r="27" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="28" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B28" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="93" t="s">
+      <c r="C28" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="94"/>
-      <c r="E28" s="94"/>
-      <c r="F28" s="94"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
       <c r="G28" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H28" s="94" t="s">
+      <c r="H28" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="I28" s="95"/>
+      <c r="I28" s="50"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B29" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="96" t="s">
+      <c r="C29" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="97"/>
-      <c r="E29" s="97"/>
-      <c r="F29" s="98"/>
+      <c r="D29" s="85"/>
+      <c r="E29" s="85"/>
+      <c r="F29" s="86"/>
       <c r="G29" s="16"/>
-      <c r="H29" s="99"/>
-      <c r="I29" s="100"/>
+      <c r="H29" s="116"/>
+      <c r="I29" s="117"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B30" s="11" t="s">
@@ -2567,8 +2683,8 @@
       <c r="E30" s="37"/>
       <c r="F30" s="38"/>
       <c r="G30" s="16"/>
-      <c r="H30" s="112"/>
-      <c r="I30" s="113"/>
+      <c r="H30" s="97"/>
+      <c r="I30" s="98"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B31" s="11" t="s">
@@ -2581,14 +2697,14 @@
       <c r="E31" s="37"/>
       <c r="F31" s="38"/>
       <c r="G31" s="16"/>
-      <c r="H31" s="112"/>
-      <c r="I31" s="113"/>
+      <c r="H31" s="97"/>
+      <c r="I31" s="98"/>
     </row>
     <row r="32" spans="2:10" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B32" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="71" t="s">
+      <c r="C32" s="63" t="s">
         <v>33</v>
       </c>
       <c r="D32" s="37"/>
@@ -2597,10 +2713,10 @@
       <c r="G32" s="16">
         <v>0.5</v>
       </c>
-      <c r="H32" s="88" t="s">
+      <c r="H32" s="127" t="s">
         <v>40</v>
       </c>
-      <c r="I32" s="76"/>
+      <c r="I32" s="100"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B33" s="11" t="s">
@@ -2615,8 +2731,8 @@
       <c r="G33" s="16">
         <v>1</v>
       </c>
-      <c r="H33" s="112"/>
-      <c r="I33" s="113"/>
+      <c r="H33" s="97"/>
+      <c r="I33" s="98"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B34" s="11" t="s">
@@ -2631,8 +2747,8 @@
       <c r="G34" s="16">
         <v>1</v>
       </c>
-      <c r="H34" s="112"/>
-      <c r="I34" s="113"/>
+      <c r="H34" s="97"/>
+      <c r="I34" s="98"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B35" s="11" t="s">
@@ -2647,8 +2763,8 @@
       <c r="G35" s="16">
         <v>1</v>
       </c>
-      <c r="H35" s="112"/>
-      <c r="I35" s="113"/>
+      <c r="H35" s="97"/>
+      <c r="I35" s="98"/>
     </row>
     <row r="36" spans="2:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B36" s="11" t="s">
@@ -2660,76 +2776,76 @@
       <c r="D36" s="37"/>
       <c r="E36" s="37"/>
       <c r="F36" s="38"/>
-      <c r="G36" s="48">
+      <c r="G36" s="75">
         <v>0.5</v>
       </c>
-      <c r="H36" s="65" t="s">
+      <c r="H36" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="I36" s="114"/>
+      <c r="I36" s="128"/>
     </row>
     <row r="37" spans="2:10" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B37" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="39" t="s">
+      <c r="C37" s="109" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="40"/>
-      <c r="E37" s="40"/>
-      <c r="F37" s="41"/>
-      <c r="G37" s="64"/>
-      <c r="H37" s="115"/>
-      <c r="I37" s="116"/>
+      <c r="D37" s="110"/>
+      <c r="E37" s="110"/>
+      <c r="F37" s="111"/>
+      <c r="G37" s="77"/>
+      <c r="H37" s="129"/>
+      <c r="I37" s="130"/>
     </row>
     <row r="38" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="39" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B39" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C39" s="93" t="s">
+      <c r="C39" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="D39" s="94"/>
-      <c r="E39" s="94"/>
-      <c r="F39" s="94"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="49"/>
       <c r="G39" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="H39" s="94" t="s">
+      <c r="H39" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="I39" s="95"/>
+      <c r="I39" s="50"/>
     </row>
     <row r="40" spans="2:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B40" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="101" t="s">
+      <c r="C40" s="118" t="s">
         <v>42</v>
       </c>
-      <c r="D40" s="102"/>
-      <c r="E40" s="102"/>
-      <c r="F40" s="103"/>
-      <c r="G40" s="107">
+      <c r="D40" s="46"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="119"/>
+      <c r="G40" s="57">
         <v>0.3</v>
       </c>
-      <c r="H40" s="108" t="s">
+      <c r="H40" s="123" t="s">
         <v>46</v>
       </c>
-      <c r="I40" s="109"/>
+      <c r="I40" s="124"/>
     </row>
     <row r="41" spans="2:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B41" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="104"/>
-      <c r="D41" s="105"/>
-      <c r="E41" s="105"/>
-      <c r="F41" s="106"/>
-      <c r="G41" s="49"/>
-      <c r="H41" s="110"/>
-      <c r="I41" s="111"/>
+      <c r="C41" s="120"/>
+      <c r="D41" s="121"/>
+      <c r="E41" s="121"/>
+      <c r="F41" s="122"/>
+      <c r="G41" s="58"/>
+      <c r="H41" s="125"/>
+      <c r="I41" s="126"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B42" s="11" t="s">
@@ -2742,14 +2858,14 @@
       <c r="E42" s="37"/>
       <c r="F42" s="38"/>
       <c r="G42" s="16"/>
-      <c r="H42" s="75"/>
-      <c r="I42" s="76"/>
+      <c r="H42" s="99"/>
+      <c r="I42" s="100"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B43" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="71" t="s">
+      <c r="C43" s="63" t="s">
         <v>43</v>
       </c>
       <c r="D43" s="37"/>
@@ -2758,14 +2874,14 @@
       <c r="G43" s="20">
         <v>1</v>
       </c>
-      <c r="H43" s="75"/>
-      <c r="I43" s="76"/>
+      <c r="H43" s="99"/>
+      <c r="I43" s="100"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B44" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C44" s="71" t="s">
+      <c r="C44" s="63" t="s">
         <v>44</v>
       </c>
       <c r="D44" s="37"/>
@@ -2774,38 +2890,38 @@
       <c r="G44" s="20">
         <v>1</v>
       </c>
-      <c r="H44" s="75"/>
-      <c r="I44" s="76"/>
+      <c r="H44" s="99"/>
+      <c r="I44" s="100"/>
     </row>
     <row r="45" spans="2:10" ht="36.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B45" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C45" s="131" t="s">
+      <c r="C45" s="91" t="s">
         <v>47</v>
       </c>
-      <c r="D45" s="132"/>
-      <c r="E45" s="132"/>
-      <c r="F45" s="132"/>
+      <c r="D45" s="92"/>
+      <c r="E45" s="92"/>
+      <c r="F45" s="92"/>
       <c r="G45" s="22"/>
-      <c r="H45" s="133"/>
-      <c r="I45" s="134"/>
+      <c r="H45" s="93"/>
+      <c r="I45" s="94"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B46" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C46" s="135" t="s">
+      <c r="C46" s="95" t="s">
         <v>51</v>
       </c>
-      <c r="D46" s="136"/>
-      <c r="E46" s="136"/>
-      <c r="F46" s="136"/>
+      <c r="D46" s="96"/>
+      <c r="E46" s="96"/>
+      <c r="F46" s="96"/>
       <c r="G46" s="22">
         <v>1</v>
       </c>
-      <c r="H46" s="112"/>
-      <c r="I46" s="113"/>
+      <c r="H46" s="97"/>
+      <c r="I46" s="98"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B47" s="11" t="s">
@@ -2820,26 +2936,26 @@
       <c r="G47" s="21">
         <v>1</v>
       </c>
-      <c r="H47" s="88"/>
-      <c r="I47" s="89"/>
+      <c r="H47" s="127"/>
+      <c r="I47" s="140"/>
     </row>
     <row r="48" spans="2:10" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B48" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C48" s="39" t="s">
+      <c r="C48" s="109" t="s">
         <v>49</v>
       </c>
-      <c r="D48" s="40"/>
-      <c r="E48" s="40"/>
-      <c r="F48" s="41"/>
+      <c r="D48" s="110"/>
+      <c r="E48" s="110"/>
+      <c r="F48" s="111"/>
       <c r="G48" s="17">
         <v>0.8</v>
       </c>
-      <c r="H48" s="86" t="s">
+      <c r="H48" s="138" t="s">
         <v>50</v>
       </c>
-      <c r="I48" s="90"/>
+      <c r="I48" s="141"/>
       <c r="J48" s="25" t="s">
         <v>57</v>
       </c>
@@ -2849,35 +2965,35 @@
       <c r="B50" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C50" s="93" t="s">
+      <c r="C50" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="D50" s="94"/>
-      <c r="E50" s="94"/>
-      <c r="F50" s="94"/>
+      <c r="D50" s="49"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="49"/>
       <c r="G50" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H50" s="94" t="s">
+      <c r="H50" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="I50" s="95"/>
+      <c r="I50" s="50"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B51" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C51" s="96" t="s">
+      <c r="C51" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="D51" s="97"/>
-      <c r="E51" s="97"/>
-      <c r="F51" s="98"/>
+      <c r="D51" s="85"/>
+      <c r="E51" s="85"/>
+      <c r="F51" s="86"/>
       <c r="G51" s="20">
         <v>1</v>
       </c>
-      <c r="H51" s="129"/>
-      <c r="I51" s="130"/>
+      <c r="H51" s="89"/>
+      <c r="I51" s="90"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B52" s="11" t="s">
@@ -2892,8 +3008,8 @@
       <c r="G52" s="20">
         <v>1</v>
       </c>
-      <c r="H52" s="72"/>
-      <c r="I52" s="73"/>
+      <c r="H52" s="41"/>
+      <c r="I52" s="42"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B53" s="11" t="s">
@@ -2906,24 +3022,24 @@
       <c r="E53" s="37"/>
       <c r="F53" s="38"/>
       <c r="G53" s="20"/>
-      <c r="H53" s="72"/>
-      <c r="I53" s="73"/>
+      <c r="H53" s="41"/>
+      <c r="I53" s="42"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B54" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C54" s="71" t="s">
+      <c r="C54" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="D54" s="91"/>
-      <c r="E54" s="91"/>
-      <c r="F54" s="92"/>
+      <c r="D54" s="64"/>
+      <c r="E54" s="64"/>
+      <c r="F54" s="65"/>
       <c r="G54" s="20">
         <v>1</v>
       </c>
-      <c r="H54" s="72"/>
-      <c r="I54" s="73"/>
+      <c r="H54" s="41"/>
+      <c r="I54" s="42"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B55" s="11" t="s">
@@ -2938,115 +3054,115 @@
       <c r="G55" s="20">
         <v>1</v>
       </c>
-      <c r="H55" s="72"/>
-      <c r="I55" s="73"/>
+      <c r="H55" s="41"/>
+      <c r="I55" s="42"/>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B56" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C56" s="71" t="s">
+      <c r="C56" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="D56" s="91"/>
-      <c r="E56" s="91"/>
-      <c r="F56" s="92"/>
+      <c r="D56" s="64"/>
+      <c r="E56" s="64"/>
+      <c r="F56" s="65"/>
       <c r="G56" s="20">
         <v>1</v>
       </c>
-      <c r="H56" s="72"/>
-      <c r="I56" s="73"/>
+      <c r="H56" s="41"/>
+      <c r="I56" s="42"/>
     </row>
     <row r="57" spans="2:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B57" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C57" s="42" t="s">
+      <c r="C57" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="44"/>
-      <c r="G57" s="48">
+      <c r="D57" s="67"/>
+      <c r="E57" s="67"/>
+      <c r="F57" s="68"/>
+      <c r="G57" s="75">
         <v>0.3</v>
       </c>
-      <c r="H57" s="65" t="s">
+      <c r="H57" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="I57" s="66"/>
+      <c r="I57" s="79"/>
     </row>
     <row r="58" spans="2:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B58" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C58" s="77"/>
-      <c r="D58" s="78"/>
-      <c r="E58" s="78"/>
-      <c r="F58" s="79"/>
-      <c r="G58" s="63"/>
-      <c r="H58" s="67"/>
-      <c r="I58" s="68"/>
+      <c r="C58" s="69"/>
+      <c r="D58" s="70"/>
+      <c r="E58" s="70"/>
+      <c r="F58" s="71"/>
+      <c r="G58" s="76"/>
+      <c r="H58" s="80"/>
+      <c r="I58" s="81"/>
     </row>
     <row r="59" spans="2:9" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B59" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C59" s="144"/>
-      <c r="D59" s="145"/>
-      <c r="E59" s="145"/>
-      <c r="F59" s="146"/>
-      <c r="G59" s="64"/>
-      <c r="H59" s="69"/>
-      <c r="I59" s="70"/>
+      <c r="C59" s="72"/>
+      <c r="D59" s="73"/>
+      <c r="E59" s="73"/>
+      <c r="F59" s="74"/>
+      <c r="G59" s="77"/>
+      <c r="H59" s="82"/>
+      <c r="I59" s="83"/>
     </row>
     <row r="60" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="61" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B61" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C61" s="93" t="s">
+      <c r="C61" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="D61" s="94"/>
-      <c r="E61" s="94"/>
-      <c r="F61" s="94"/>
+      <c r="D61" s="49"/>
+      <c r="E61" s="49"/>
+      <c r="F61" s="49"/>
       <c r="G61" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="H61" s="94" t="s">
+      <c r="H61" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="I61" s="95"/>
+      <c r="I61" s="50"/>
     </row>
     <row r="62" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B62" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C62" s="137" t="s">
+      <c r="C62" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="D62" s="138"/>
-      <c r="E62" s="138"/>
-      <c r="F62" s="139"/>
-      <c r="G62" s="107">
+      <c r="D62" s="52"/>
+      <c r="E62" s="52"/>
+      <c r="F62" s="53"/>
+      <c r="G62" s="57">
         <v>0.3</v>
       </c>
-      <c r="H62" s="140" t="s">
+      <c r="H62" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="I62" s="141"/>
+      <c r="I62" s="60"/>
     </row>
     <row r="63" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B63" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C63" s="45"/>
-      <c r="D63" s="46"/>
-      <c r="E63" s="46"/>
-      <c r="F63" s="47"/>
-      <c r="G63" s="49"/>
-      <c r="H63" s="142"/>
-      <c r="I63" s="143"/>
+      <c r="C63" s="54"/>
+      <c r="D63" s="55"/>
+      <c r="E63" s="55"/>
+      <c r="F63" s="56"/>
+      <c r="G63" s="58"/>
+      <c r="H63" s="61"/>
+      <c r="I63" s="62"/>
     </row>
     <row r="64" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B64" s="11" t="s">
@@ -3059,27 +3175,27 @@
       <c r="E64" s="37"/>
       <c r="F64" s="38"/>
       <c r="G64" s="24"/>
-      <c r="H64" s="151"/>
-      <c r="I64" s="152"/>
+      <c r="H64" s="43"/>
+      <c r="I64" s="44"/>
     </row>
     <row r="65" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B65" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C65" s="42" t="s">
+      <c r="C65" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="D65" s="43"/>
-      <c r="E65" s="43"/>
-      <c r="F65" s="44"/>
-      <c r="G65" s="48">
+      <c r="D65" s="67"/>
+      <c r="E65" s="67"/>
+      <c r="F65" s="68"/>
+      <c r="G65" s="75">
         <v>1</v>
       </c>
-      <c r="H65" s="80" t="s">
+      <c r="H65" s="132" t="s">
         <v>68</v>
       </c>
-      <c r="I65" s="81"/>
-      <c r="L65" s="71" t="s">
+      <c r="I65" s="133"/>
+      <c r="L65" s="63" t="s">
         <v>62</v>
       </c>
       <c r="M65" s="37"/>
@@ -3090,13 +3206,13 @@
       <c r="B66" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C66" s="77"/>
-      <c r="D66" s="78"/>
-      <c r="E66" s="78"/>
-      <c r="F66" s="79"/>
-      <c r="G66" s="63"/>
-      <c r="H66" s="82"/>
-      <c r="I66" s="83"/>
+      <c r="C66" s="69"/>
+      <c r="D66" s="70"/>
+      <c r="E66" s="70"/>
+      <c r="F66" s="71"/>
+      <c r="G66" s="76"/>
+      <c r="H66" s="134"/>
+      <c r="I66" s="135"/>
       <c r="L66" s="36" t="s">
         <v>65</v>
       </c>
@@ -3108,13 +3224,13 @@
       <c r="B67" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C67" s="77"/>
-      <c r="D67" s="78"/>
-      <c r="E67" s="78"/>
-      <c r="F67" s="79"/>
-      <c r="G67" s="63"/>
-      <c r="H67" s="82"/>
-      <c r="I67" s="83"/>
+      <c r="C67" s="69"/>
+      <c r="D67" s="70"/>
+      <c r="E67" s="70"/>
+      <c r="F67" s="71"/>
+      <c r="G67" s="76"/>
+      <c r="H67" s="134"/>
+      <c r="I67" s="135"/>
       <c r="L67" s="36" t="s">
         <v>65</v>
       </c>
@@ -3126,13 +3242,13 @@
       <c r="B68" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C68" s="77"/>
-      <c r="D68" s="78"/>
-      <c r="E68" s="78"/>
-      <c r="F68" s="79"/>
-      <c r="G68" s="63"/>
-      <c r="H68" s="82"/>
-      <c r="I68" s="83"/>
+      <c r="C68" s="69"/>
+      <c r="D68" s="70"/>
+      <c r="E68" s="70"/>
+      <c r="F68" s="71"/>
+      <c r="G68" s="76"/>
+      <c r="H68" s="134"/>
+      <c r="I68" s="135"/>
       <c r="L68" s="36" t="s">
         <v>63</v>
       </c>
@@ -3144,13 +3260,13 @@
       <c r="B69" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C69" s="45"/>
-      <c r="D69" s="46"/>
-      <c r="E69" s="46"/>
-      <c r="F69" s="47"/>
-      <c r="G69" s="49"/>
-      <c r="H69" s="84"/>
-      <c r="I69" s="85"/>
+      <c r="C69" s="54"/>
+      <c r="D69" s="55"/>
+      <c r="E69" s="55"/>
+      <c r="F69" s="56"/>
+      <c r="G69" s="58"/>
+      <c r="H69" s="136"/>
+      <c r="I69" s="137"/>
       <c r="L69" s="36" t="s">
         <v>64</v>
       </c>
@@ -3162,40 +3278,40 @@
       <c r="B70" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C70" s="39" t="s">
+      <c r="C70" s="109" t="s">
         <v>69</v>
       </c>
-      <c r="D70" s="40"/>
-      <c r="E70" s="40"/>
-      <c r="F70" s="41"/>
+      <c r="D70" s="110"/>
+      <c r="E70" s="110"/>
+      <c r="F70" s="111"/>
       <c r="G70" s="17">
         <v>0.5</v>
       </c>
-      <c r="H70" s="86" t="s">
+      <c r="H70" s="138" t="s">
         <v>70</v>
       </c>
-      <c r="I70" s="87"/>
-      <c r="L70" s="39" t="s">
+      <c r="I70" s="139"/>
+      <c r="L70" s="109" t="s">
         <v>64</v>
       </c>
-      <c r="M70" s="40"/>
-      <c r="N70" s="40"/>
-      <c r="O70" s="41"/>
+      <c r="M70" s="110"/>
+      <c r="N70" s="110"/>
+      <c r="O70" s="111"/>
     </row>
     <row r="71" spans="2:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B71" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="C71" s="153" t="s">
+      <c r="C71" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="D71" s="102"/>
-      <c r="E71" s="102"/>
-      <c r="F71" s="102"/>
-      <c r="H71" s="154" t="s">
+      <c r="D71" s="46"/>
+      <c r="E71" s="46"/>
+      <c r="F71" s="46"/>
+      <c r="H71" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="I71" s="154"/>
+      <c r="I71" s="47"/>
       <c r="J71" t="s">
         <v>74</v>
       </c>
@@ -3205,37 +3321,37 @@
       <c r="B74" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C74" s="93" t="s">
+      <c r="C74" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="D74" s="94"/>
-      <c r="E74" s="94"/>
-      <c r="F74" s="94"/>
+      <c r="D74" s="49"/>
+      <c r="E74" s="49"/>
+      <c r="F74" s="49"/>
       <c r="G74" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="H74" s="94" t="s">
+      <c r="H74" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="I74" s="95"/>
+      <c r="I74" s="50"/>
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B75" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C75" s="96" t="s">
+      <c r="C75" s="84" t="s">
         <v>77</v>
       </c>
-      <c r="D75" s="97"/>
-      <c r="E75" s="97"/>
-      <c r="F75" s="98"/>
+      <c r="D75" s="85"/>
+      <c r="E75" s="85"/>
+      <c r="F75" s="86"/>
       <c r="G75" s="27">
         <v>0</v>
       </c>
-      <c r="H75" s="147" t="s">
+      <c r="H75" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="I75" s="148"/>
+      <c r="I75" s="88"/>
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B76" s="11" t="s">
@@ -3250,10 +3366,10 @@
       <c r="G76" s="27">
         <v>0</v>
       </c>
-      <c r="H76" s="149" t="s">
+      <c r="H76" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="I76" s="150"/>
+      <c r="I76" s="40"/>
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B77" s="11" t="s">
@@ -3266,14 +3382,14 @@
       <c r="E77" s="37"/>
       <c r="F77" s="38"/>
       <c r="G77" s="27"/>
-      <c r="H77" s="72"/>
-      <c r="I77" s="73"/>
+      <c r="H77" s="41"/>
+      <c r="I77" s="42"/>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B78" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C78" s="71" t="s">
+      <c r="C78" s="63" t="s">
         <v>79</v>
       </c>
       <c r="D78" s="37"/>
@@ -3282,8 +3398,8 @@
       <c r="G78" s="27">
         <v>1</v>
       </c>
-      <c r="H78" s="72"/>
-      <c r="I78" s="73"/>
+      <c r="H78" s="41"/>
+      <c r="I78" s="42"/>
       <c r="L78" s="36" t="s">
         <v>80</v>
       </c>
@@ -3295,17 +3411,17 @@
       <c r="B79" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C79" s="42" t="s">
+      <c r="C79" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="D79" s="43"/>
-      <c r="E79" s="43"/>
-      <c r="F79" s="44"/>
-      <c r="G79" s="48">
+      <c r="D79" s="67"/>
+      <c r="E79" s="67"/>
+      <c r="F79" s="68"/>
+      <c r="G79" s="75">
         <v>1</v>
       </c>
-      <c r="H79" s="50"/>
-      <c r="I79" s="51"/>
+      <c r="H79" s="143"/>
+      <c r="I79" s="144"/>
       <c r="L79" s="36" t="s">
         <v>81</v>
       </c>
@@ -3317,154 +3433,131 @@
       <c r="B80" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C80" s="45"/>
-      <c r="D80" s="46"/>
-      <c r="E80" s="46"/>
-      <c r="F80" s="47"/>
-      <c r="G80" s="49"/>
-      <c r="H80" s="52"/>
-      <c r="I80" s="53"/>
-      <c r="L80" s="39" t="s">
+      <c r="C80" s="54"/>
+      <c r="D80" s="55"/>
+      <c r="E80" s="55"/>
+      <c r="F80" s="56"/>
+      <c r="G80" s="58"/>
+      <c r="H80" s="145"/>
+      <c r="I80" s="146"/>
+      <c r="L80" s="109" t="s">
         <v>82</v>
       </c>
-      <c r="M80" s="40"/>
-      <c r="N80" s="40"/>
-      <c r="O80" s="41"/>
+      <c r="M80" s="110"/>
+      <c r="N80" s="110"/>
+      <c r="O80" s="111"/>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B81" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C81" s="54" t="s">
+      <c r="C81" s="147" t="s">
         <v>65</v>
       </c>
-      <c r="D81" s="55"/>
-      <c r="E81" s="55"/>
-      <c r="F81" s="56"/>
-      <c r="G81" s="48">
+      <c r="D81" s="148"/>
+      <c r="E81" s="148"/>
+      <c r="F81" s="149"/>
+      <c r="G81" s="75">
         <v>0.7</v>
       </c>
-      <c r="H81" s="65" t="s">
+      <c r="H81" s="78" t="s">
         <v>85</v>
       </c>
-      <c r="I81" s="66"/>
+      <c r="I81" s="79"/>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B82" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C82" s="57"/>
-      <c r="D82" s="58"/>
-      <c r="E82" s="58"/>
-      <c r="F82" s="59"/>
-      <c r="G82" s="63"/>
-      <c r="H82" s="67"/>
-      <c r="I82" s="68"/>
+      <c r="C82" s="150"/>
+      <c r="D82" s="151"/>
+      <c r="E82" s="151"/>
+      <c r="F82" s="152"/>
+      <c r="G82" s="76"/>
+      <c r="H82" s="80"/>
+      <c r="I82" s="81"/>
     </row>
     <row r="83" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B83" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C83" s="60"/>
-      <c r="D83" s="61"/>
-      <c r="E83" s="61"/>
-      <c r="F83" s="62"/>
-      <c r="G83" s="64"/>
-      <c r="H83" s="69"/>
-      <c r="I83" s="70"/>
+      <c r="C83" s="153"/>
+      <c r="D83" s="154"/>
+      <c r="E83" s="154"/>
+      <c r="F83" s="155"/>
+      <c r="G83" s="77"/>
+      <c r="H83" s="82"/>
+      <c r="I83" s="83"/>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B84" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="C84" s="35" t="s">
+      <c r="C84" s="142" t="s">
         <v>87</v>
       </c>
-      <c r="D84" s="35"/>
-      <c r="E84" s="35"/>
-      <c r="F84" s="35"/>
+      <c r="D84" s="142"/>
+      <c r="E84" s="142"/>
+      <c r="F84" s="142"/>
       <c r="G84" s="1"/>
-      <c r="H84" s="35" t="s">
+      <c r="H84" s="142" t="s">
         <v>88</v>
       </c>
-      <c r="I84" s="35"/>
+      <c r="I84" s="142"/>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B85" s="31"/>
-      <c r="C85" s="74" t="s">
+      <c r="C85" s="131" t="s">
         <v>89</v>
       </c>
-      <c r="D85" s="74"/>
-      <c r="E85" s="74"/>
-      <c r="F85" s="74"/>
-      <c r="H85" s="74" t="s">
+      <c r="D85" s="131"/>
+      <c r="E85" s="131"/>
+      <c r="F85" s="131"/>
+      <c r="H85" s="131" t="s">
         <v>88</v>
       </c>
-      <c r="I85" s="74"/>
+      <c r="I85" s="131"/>
     </row>
     <row r="95" spans="2:9" ht="54" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="121">
-    <mergeCell ref="C76:F76"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="C77:F77"/>
-    <mergeCell ref="H77:I77"/>
-    <mergeCell ref="C64:F64"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="C71:F71"/>
-    <mergeCell ref="H71:I71"/>
-    <mergeCell ref="C74:F74"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="C62:F63"/>
-    <mergeCell ref="G62:G63"/>
-    <mergeCell ref="H62:I63"/>
-    <mergeCell ref="C56:F56"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="C57:F59"/>
-    <mergeCell ref="G57:G59"/>
-    <mergeCell ref="H57:I59"/>
-    <mergeCell ref="C75:F75"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="C50:F50"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="C51:F51"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="C52:F52"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="C61:F61"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="C45:F45"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="C46:F46"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="C42:F42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="C43:F43"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H5:I13"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="C84:F84"/>
+    <mergeCell ref="H84:I84"/>
+    <mergeCell ref="L78:O78"/>
+    <mergeCell ref="L79:O79"/>
+    <mergeCell ref="L80:O80"/>
+    <mergeCell ref="C79:F80"/>
+    <mergeCell ref="G79:G80"/>
+    <mergeCell ref="H79:I80"/>
+    <mergeCell ref="C81:F83"/>
+    <mergeCell ref="G81:G83"/>
+    <mergeCell ref="H81:I83"/>
+    <mergeCell ref="C78:F78"/>
+    <mergeCell ref="H78:I78"/>
+    <mergeCell ref="C85:F85"/>
+    <mergeCell ref="H85:I85"/>
+    <mergeCell ref="C44:F44"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="L70:O70"/>
+    <mergeCell ref="C65:F69"/>
+    <mergeCell ref="G65:G69"/>
+    <mergeCell ref="H65:I69"/>
+    <mergeCell ref="L65:O65"/>
+    <mergeCell ref="L66:O66"/>
+    <mergeCell ref="L67:O67"/>
+    <mergeCell ref="L68:O68"/>
+    <mergeCell ref="L69:O69"/>
+    <mergeCell ref="C70:F70"/>
+    <mergeCell ref="H70:I70"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="C53:F53"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="C54:F54"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="C55:F55"/>
     <mergeCell ref="C28:F28"/>
     <mergeCell ref="H28:I28"/>
     <mergeCell ref="C29:F29"/>
@@ -3489,43 +3582,66 @@
     <mergeCell ref="G36:G37"/>
     <mergeCell ref="H36:I37"/>
     <mergeCell ref="C39:F39"/>
-    <mergeCell ref="C85:F85"/>
-    <mergeCell ref="H85:I85"/>
-    <mergeCell ref="C44:F44"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="L70:O70"/>
-    <mergeCell ref="C65:F69"/>
-    <mergeCell ref="G65:G69"/>
-    <mergeCell ref="H65:I69"/>
-    <mergeCell ref="L65:O65"/>
-    <mergeCell ref="L66:O66"/>
-    <mergeCell ref="L67:O67"/>
-    <mergeCell ref="L68:O68"/>
-    <mergeCell ref="L69:O69"/>
-    <mergeCell ref="C70:F70"/>
-    <mergeCell ref="H70:I70"/>
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="C53:F53"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="C54:F54"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="C55:F55"/>
-    <mergeCell ref="C84:F84"/>
-    <mergeCell ref="H84:I84"/>
-    <mergeCell ref="L78:O78"/>
-    <mergeCell ref="L79:O79"/>
-    <mergeCell ref="L80:O80"/>
-    <mergeCell ref="C79:F80"/>
-    <mergeCell ref="G79:G80"/>
-    <mergeCell ref="H79:I80"/>
-    <mergeCell ref="C81:F83"/>
-    <mergeCell ref="G81:G83"/>
-    <mergeCell ref="H81:I83"/>
-    <mergeCell ref="C78:F78"/>
-    <mergeCell ref="H78:I78"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H5:I13"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="C46:F46"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="C42:F42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="C50:F50"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="C52:F52"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="C61:F61"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="C62:F63"/>
+    <mergeCell ref="G62:G63"/>
+    <mergeCell ref="H62:I63"/>
+    <mergeCell ref="C56:F56"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="C57:F59"/>
+    <mergeCell ref="G57:G59"/>
+    <mergeCell ref="H57:I59"/>
+    <mergeCell ref="C75:F75"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="C76:F76"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="C77:F77"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="C64:F64"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="C71:F71"/>
+    <mergeCell ref="H71:I71"/>
+    <mergeCell ref="C74:F74"/>
+    <mergeCell ref="H74:I74"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3535,16 +3651,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{813EEE76-69D4-4EE1-98FD-50720CEB1426}">
-  <dimension ref="B2:I23"/>
+  <dimension ref="B2:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:F12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="14.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.796875" customWidth="1"/>
+    <col min="5" max="5" width="10.59765625" customWidth="1"/>
+    <col min="6" max="6" width="20.09765625" customWidth="1"/>
     <col min="9" max="9" width="28.69921875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3553,35 +3670,35 @@
       <c r="B3" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="93" t="s">
+      <c r="C3" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
       <c r="G3" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="94" t="s">
+      <c r="H3" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="95"/>
+      <c r="I3" s="50"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="96" t="s">
+      <c r="C4" s="84" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="97"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="98"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="86"/>
       <c r="G4" s="30">
         <v>1</v>
       </c>
-      <c r="H4" s="129"/>
-      <c r="I4" s="130"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="90"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B5" s="11" t="s">
@@ -3596,8 +3713,8 @@
       <c r="G5" s="30">
         <v>1</v>
       </c>
-      <c r="H5" s="72"/>
-      <c r="I5" s="73"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="42"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B6" s="11" t="s">
@@ -3610,24 +3727,24 @@
       <c r="E6" s="37"/>
       <c r="F6" s="38"/>
       <c r="G6" s="30"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="73"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="42"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="71" t="s">
+      <c r="C7" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="D7" s="91"/>
-      <c r="E7" s="91"/>
-      <c r="F7" s="92"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="65"/>
       <c r="G7" s="30">
         <v>1</v>
       </c>
-      <c r="H7" s="72"/>
-      <c r="I7" s="73"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="42"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B8" s="11" t="s">
@@ -3640,72 +3757,72 @@
       <c r="E8" s="37"/>
       <c r="F8" s="38"/>
       <c r="G8" s="30"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="73"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="42"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="71" t="s">
+      <c r="C9" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="D9" s="91"/>
-      <c r="E9" s="91"/>
-      <c r="F9" s="92"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="65"/>
       <c r="G9" s="30"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="73"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="42"/>
     </row>
     <row r="10" spans="2:9" ht="54" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="71" t="s">
+      <c r="C10" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="D10" s="91"/>
-      <c r="E10" s="91"/>
-      <c r="F10" s="92"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="65"/>
       <c r="G10" s="22">
         <v>0.8</v>
       </c>
-      <c r="H10" s="161" t="s">
+      <c r="H10" s="158" t="s">
         <v>98</v>
       </c>
-      <c r="I10" s="162"/>
+      <c r="I10" s="159"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="71" t="s">
+      <c r="C11" s="63" t="s">
         <v>96</v>
       </c>
-      <c r="D11" s="91"/>
-      <c r="E11" s="91"/>
-      <c r="F11" s="92"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="65"/>
       <c r="G11" s="22">
         <v>1</v>
       </c>
-      <c r="H11" s="157"/>
-      <c r="I11" s="158"/>
+      <c r="H11" s="160"/>
+      <c r="I11" s="161"/>
     </row>
     <row r="12" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B12" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="D12" s="155"/>
-      <c r="E12" s="155"/>
-      <c r="F12" s="156"/>
+      <c r="D12" s="156"/>
+      <c r="E12" s="156"/>
+      <c r="F12" s="157"/>
       <c r="G12" s="17">
         <v>1</v>
       </c>
-      <c r="H12" s="159"/>
-      <c r="I12" s="160"/>
+      <c r="H12" s="162"/>
+      <c r="I12" s="163"/>
     </row>
     <row r="13" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C13" s="32"/>
@@ -3715,35 +3832,35 @@
     </row>
     <row r="14" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B14" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="C14" s="93" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="94"/>
-      <c r="E14" s="94"/>
-      <c r="F14" s="94"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
       <c r="G14" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="94" t="s">
+      <c r="H14" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="I14" s="95"/>
+      <c r="I14" s="50"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B15" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="96" t="s">
+      <c r="C15" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="97"/>
-      <c r="E15" s="97"/>
-      <c r="F15" s="98"/>
+      <c r="D15" s="85"/>
+      <c r="E15" s="85"/>
+      <c r="F15" s="86"/>
       <c r="G15" s="34"/>
-      <c r="H15" s="129"/>
-      <c r="I15" s="130"/>
+      <c r="H15" s="89"/>
+      <c r="I15" s="90"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B16" s="11" t="s">
@@ -3756,8 +3873,8 @@
       <c r="E16" s="37"/>
       <c r="F16" s="38"/>
       <c r="G16" s="34"/>
-      <c r="H16" s="72"/>
-      <c r="I16" s="73"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="42"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B17" s="11" t="s">
@@ -3770,119 +3887,250 @@
       <c r="E17" s="37"/>
       <c r="F17" s="38"/>
       <c r="G17" s="34"/>
-      <c r="H17" s="72"/>
-      <c r="I17" s="73"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="42"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B18" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="71" t="s">
-        <v>99</v>
-      </c>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="73"/>
+      <c r="C18" s="174" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="175"/>
+      <c r="E18" s="175"/>
+      <c r="F18" s="176"/>
+      <c r="G18" s="75">
+        <v>1</v>
+      </c>
+      <c r="H18" s="143"/>
+      <c r="I18" s="144"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B19" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="72"/>
-      <c r="I19" s="73"/>
+      <c r="C19" s="193"/>
+      <c r="D19" s="194"/>
+      <c r="E19" s="194"/>
+      <c r="F19" s="195"/>
+      <c r="G19" s="76"/>
+      <c r="H19" s="164"/>
+      <c r="I19" s="165"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B20" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="72"/>
-      <c r="I20" s="73"/>
+      <c r="C20" s="193"/>
+      <c r="D20" s="194"/>
+      <c r="E20" s="194"/>
+      <c r="F20" s="195"/>
+      <c r="G20" s="76"/>
+      <c r="H20" s="164"/>
+      <c r="I20" s="165"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B21" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="72"/>
-      <c r="I21" s="73"/>
+      <c r="C21" s="120"/>
+      <c r="D21" s="121"/>
+      <c r="E21" s="121"/>
+      <c r="F21" s="122"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="145"/>
+      <c r="I21" s="146"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B22" s="11" t="s">
         <v>14</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D22" s="37"/>
       <c r="E22" s="37"/>
       <c r="F22" s="38"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="119"/>
-      <c r="I22" s="120"/>
+      <c r="G22" s="34">
+        <v>1</v>
+      </c>
+      <c r="H22" s="114"/>
+      <c r="I22" s="115"/>
     </row>
     <row r="23" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B23" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="109" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" s="110"/>
+      <c r="E23" s="110"/>
+      <c r="F23" s="111"/>
+      <c r="G23" s="17">
+        <v>1</v>
+      </c>
+      <c r="H23" s="112"/>
+      <c r="I23" s="113"/>
+    </row>
+    <row r="24" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="25" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B25" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="117"/>
-      <c r="I23" s="118"/>
+      <c r="C25" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" s="50"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B26" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="166" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="119"/>
+      <c r="G26" s="167"/>
+      <c r="H26" s="168"/>
+      <c r="I26" s="169"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B27" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="120"/>
+      <c r="D27" s="121"/>
+      <c r="E27" s="121"/>
+      <c r="F27" s="122"/>
+      <c r="G27" s="170"/>
+      <c r="H27" s="171"/>
+      <c r="I27" s="172"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B28" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="173"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="40"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B29" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="63" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="64"/>
+      <c r="E29" s="64"/>
+      <c r="F29" s="65"/>
+      <c r="G29" s="173"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="40"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B30" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="174" t="s">
+        <v>106</v>
+      </c>
+      <c r="D30" s="175"/>
+      <c r="E30" s="175"/>
+      <c r="F30" s="176"/>
+      <c r="G30" s="177"/>
+      <c r="H30" s="178"/>
+      <c r="I30" s="179"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B31" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="120"/>
+      <c r="D31" s="121"/>
+      <c r="E31" s="121"/>
+      <c r="F31" s="122"/>
+      <c r="G31" s="170"/>
+      <c r="H31" s="171"/>
+      <c r="I31" s="172"/>
+    </row>
+    <row r="32" spans="2:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="180" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" s="181"/>
+      <c r="E32" s="181"/>
+      <c r="F32" s="182"/>
+      <c r="G32" s="177"/>
+      <c r="H32" s="78"/>
+      <c r="I32" s="128"/>
+    </row>
+    <row r="33" spans="2:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B33" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="183"/>
+      <c r="D33" s="184"/>
+      <c r="E33" s="184"/>
+      <c r="F33" s="185"/>
+      <c r="G33" s="186"/>
+      <c r="H33" s="187"/>
+      <c r="I33" s="188"/>
+    </row>
+    <row r="34" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B34" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="189"/>
+      <c r="D34" s="190"/>
+      <c r="E34" s="190"/>
+      <c r="F34" s="191"/>
+      <c r="G34" s="192"/>
+      <c r="H34" s="129"/>
+      <c r="I34" s="130"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
+  <mergeCells count="50">
+    <mergeCell ref="C30:F31"/>
+    <mergeCell ref="C32:F34"/>
+    <mergeCell ref="G32:G34"/>
+    <mergeCell ref="H32:I34"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="H30:I31"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="C26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:I27"/>
+    <mergeCell ref="C18:F21"/>
+    <mergeCell ref="G18:G21"/>
+    <mergeCell ref="H18:I21"/>
     <mergeCell ref="C22:F22"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="C23:F23"/>
@@ -3893,15 +4141,32 @@
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="H16:I16"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>